<commit_message>
- Trim cells in excel
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Python\simple-snr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABD36AD-A8D8-406D-9F55-E3B2E25FA35D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32442239-DAFC-47A2-AEEF-BCAFD17833B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,16 +39,16 @@
     <t>string 1</t>
   </si>
   <si>
-    <t>long long something</t>
-  </si>
-  <si>
-    <t>xx</t>
-  </si>
-  <si>
     <t>HoHoHo</t>
   </si>
   <si>
     <t>Me40</t>
+  </si>
+  <si>
+    <t>ķųųųų</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   long long something   </t>
   </si>
 </sst>
 </file>
@@ -369,7 +369,7 @@
   <dimension ref="A2:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -385,7 +385,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -398,13 +398,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- In/Out file to UTF8 bugfix
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Python\simple-snr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32442239-DAFC-47A2-AEEF-BCAFD17833B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC3356A-FFF1-43F0-9262-4887BCAF928B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="23040" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>string 2</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t xml:space="preserve">   long long something   </t>
+  </si>
+  <si>
+    <t>мечо е номер едно</t>
+  </si>
+  <si>
+    <t>ала бала</t>
   </si>
 </sst>
 </file>
@@ -366,15 +372,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C4"/>
+  <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -407,6 +414,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>